<commit_message>
minor changes + comments
</commit_message>
<xml_diff>
--- a/input-files/data.xlsx
+++ b/input-files/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Anastasia\Documents\Uni\bachelor\science\degree thesis\code\input-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EA65178-AED0-452A-82D4-C31C36BFE616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C11CD6-2F5E-463E-84B3-8C996B561432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15465" yWindow="120" windowWidth="13350" windowHeight="14835" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15660" windowHeight="14835" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equipment" sheetId="1" r:id="rId1"/>
@@ -39688,9 +39688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -39778,207 +39776,207 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5">
-        <v>200</v>
+        <v>14800</v>
       </c>
       <c r="D5" t="s">
         <v>43</v>
       </c>
       <c r="E5">
-        <v>3033</v>
+        <v>4524</v>
       </c>
       <c r="F5" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C6">
-        <v>4000</v>
+        <v>14800</v>
       </c>
       <c r="D6" t="s">
         <v>43</v>
       </c>
       <c r="E6">
-        <v>4224</v>
+        <v>4524</v>
       </c>
       <c r="F6" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C7">
-        <v>15000</v>
+        <v>200</v>
       </c>
       <c r="D7" t="s">
         <v>43</v>
       </c>
       <c r="E7">
-        <v>7579</v>
+        <v>3033</v>
       </c>
       <c r="F7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C8">
-        <v>600</v>
+        <v>4000</v>
       </c>
       <c r="D8" t="s">
         <v>43</v>
       </c>
       <c r="E8">
-        <v>90423</v>
+        <v>4224</v>
       </c>
       <c r="F8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C9">
-        <v>1333</v>
+        <v>5000</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
       </c>
       <c r="E9">
-        <v>1085</v>
+        <v>5280</v>
       </c>
       <c r="F9" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C10">
-        <v>600</v>
+        <v>15000</v>
       </c>
       <c r="D10" t="s">
         <v>43</v>
       </c>
       <c r="E10">
-        <v>90423</v>
+        <v>7579</v>
       </c>
       <c r="F10" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C11">
-        <v>600</v>
+        <v>15000</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
       </c>
       <c r="E11">
-        <v>90423</v>
+        <v>7579</v>
       </c>
       <c r="F11" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C12">
-        <v>5000</v>
+        <v>600</v>
       </c>
       <c r="D12" t="s">
         <v>43</v>
       </c>
       <c r="E12">
-        <v>5280</v>
+        <v>90423</v>
       </c>
       <c r="F12" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C13">
-        <v>14800</v>
+        <v>600</v>
       </c>
       <c r="D13" t="s">
         <v>43</v>
       </c>
       <c r="E13">
-        <v>4524</v>
+        <v>90423</v>
       </c>
       <c r="F13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C14">
-        <v>14800</v>
+        <v>600</v>
       </c>
       <c r="D14" t="s">
         <v>43</v>
       </c>
       <c r="E14">
-        <v>4524</v>
+        <v>90423</v>
       </c>
       <c r="F14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>174</v>
@@ -39993,32 +39991,33 @@
         <v>1085</v>
       </c>
       <c r="F15" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C16">
-        <v>15000</v>
+        <v>1333</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
       </c>
       <c r="E16">
-        <v>7579</v>
+        <v>1085</v>
       </c>
       <c r="F16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F16">
-    <sortCondition ref="A2:A16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F18">
+    <sortCondition ref="B2:B18"/>
+    <sortCondition ref="F2:F18"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -43835,7 +43834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E901"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>